<commit_message>
Against audit NC 30 : revised the checklist
for project audit.
</commit_message>
<xml_diff>
--- a/Support/Quality Assurance/CHKL_AUDITT.xlsx
+++ b/Support/Quality Assurance/CHKL_AUDITT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
   <si>
     <t>S. No</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Audit Checklist for Validation Phase End and Closure</t>
   </si>
   <si>
-    <t>Have the requirement changes requested been approved and agreed to formally? Has the Change request log been properly updated?</t>
-  </si>
-  <si>
     <t>Has the impact of those changes over the project's products been analyzed?</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Is the decision arrived at using DAR clearly stated and use sound judgment?</t>
   </si>
   <si>
-    <t>Have the integration test cases been reviewed and the defects logged?</t>
-  </si>
-  <si>
     <t>Has the milestone review of the phase end been conducted with the senior management?</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>Has the test Plan been prepared?</t>
   </si>
   <si>
-    <t>Major Non-Conformance/ Minor Non-Conformance/ Observation</t>
-  </si>
-  <si>
     <t>Log ID</t>
   </si>
   <si>
@@ -300,9 +291,6 @@
     <t>Has the preliminary effort been estimated at project start?</t>
   </si>
   <si>
-    <t>Are the skill matrix and project resource plan in sync?</t>
-  </si>
-  <si>
     <t>Has the Complexity factor been determined appropriately using all relevant factors?</t>
   </si>
   <si>
@@ -312,9 +300,6 @@
     <t>Does the training plan cover the training activities adequately such as trainer's name, duration , audiences etc.</t>
   </si>
   <si>
-    <t>Are the project learning in project learning database logged, actionable and specific?</t>
-  </si>
-  <si>
     <t>Have the proposed tailorings been approved by the PEG? Are tailoring approver and requester independent?</t>
   </si>
   <si>
@@ -381,15 +366,9 @@
     <t>Has the validation report been issued?</t>
   </si>
   <si>
-    <t>Have all the minor NCs of previous stage closed?</t>
-  </si>
-  <si>
     <t>Project Audit Checklist</t>
   </si>
   <si>
-    <t>Have all logs been updated on sharepoint?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Has/Have the Customer Inputs been verified for adequacy and completeness by the project manager? </t>
   </si>
   <si>
@@ -408,12 +387,6 @@
     <t>Have the clarifications sought from the customer been logged and tracked regularly?</t>
   </si>
   <si>
-    <t>Have the review findings been logged in the Review and Testing defects log?</t>
-  </si>
-  <si>
-    <t>Has the RTT been reviewed by the Project manager and the findings logged in the Review and Testing defects log? Have the findings been closed suitably?</t>
-  </si>
-  <si>
     <t>Have all the related artifacts such as the RTT, FS etc been placed under configuration control?</t>
   </si>
   <si>
@@ -423,18 +396,9 @@
     <t>Have the actions required for contingency and mitigation of the identified risks been properly listed?</t>
   </si>
   <si>
-    <t>Have the review findings of the plan been logged in the Review and Testing Defects log?</t>
-  </si>
-  <si>
-    <t>Have the review findings of the schedule and the risk matrix been logged in the Review and Testing Defects log?</t>
-  </si>
-  <si>
     <t>Is the rationale to modify the calculated design and implementation effort documented and satisfactory?</t>
   </si>
   <si>
-    <t>Have the appropriate number of team meetings been conducted, documented and archived? Do they cover all planning parameters including project measures and issue logs?</t>
-  </si>
-  <si>
     <t>Are all action items derived using discussions?</t>
   </si>
   <si>
@@ -444,9 +408,6 @@
     <t>Are all the external interfaces designed in the Design phase clearly traceable and marked as such in the functional specification?</t>
   </si>
   <si>
-    <t>Have the findings of the reviews conducted logged in Review and Testing Defects log?</t>
-  </si>
-  <si>
     <t>Has the design documents been reviewed with respect to requirement? (QA should sample at least one requirement and try tracking its design)</t>
   </si>
   <si>
@@ -459,33 +420,18 @@
     <t>Has DAR been applied appropriately for critical design decisions? (If DAR applied)</t>
   </si>
   <si>
-    <t>Have the findings of the reviews conducted logged in review and testing defects log?</t>
-  </si>
-  <si>
     <t>Have the Test cases been developed?</t>
   </si>
   <si>
-    <t>Has testing been conducted and the findings logged?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Have the requirement changes requested been approved and agreed to formally? </t>
   </si>
   <si>
-    <t>Have the integration steps been verified? Have the defects been logged in the Review and Testing Defects log?</t>
-  </si>
-  <si>
     <t>Are all action items derived using discussions been noted in the MOM?</t>
   </si>
   <si>
     <t>Has the updated plan been reviewed and approved?</t>
   </si>
   <si>
-    <t>Have the above been reviewed and defecs logged?</t>
-  </si>
-  <si>
-    <t>Has the product been validated and the defects logged?</t>
-  </si>
-  <si>
     <t>Is configuration auditor independent of the project team?</t>
   </si>
   <si>
@@ -498,10 +444,58 @@
     <t>Has the approved plan intimation mail been done to all relevant stakeholders?</t>
   </si>
   <si>
-    <t>Template Version - 4</t>
-  </si>
-  <si>
     <t>Has  the defects analysis done?</t>
+  </si>
+  <si>
+    <t>Template Version - 5</t>
+  </si>
+  <si>
+    <t>Have the review findings been logged in the Incident Management?</t>
+  </si>
+  <si>
+    <t>Has the RTT been reviewed by the Project manager and the findings logged in the Incident Management? Have the findings been closed suitably?</t>
+  </si>
+  <si>
+    <t>Have all logs been updated on GIL.ef?</t>
+  </si>
+  <si>
+    <t>Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation</t>
+  </si>
+  <si>
+    <t>Have the review findings of the plan been logged in the Incident Management?</t>
+  </si>
+  <si>
+    <t>Are the talent maps and gaps identified?</t>
+  </si>
+  <si>
+    <t>Have the appropriate number of team meetings been conducted, documented and archived? Do they cover all planning parameters including project measures and issues?</t>
+  </si>
+  <si>
+    <t>Have all the non-functional NCs of previous stage closed?</t>
+  </si>
+  <si>
+    <t>Have the findings of the reviews conducted logged in Incident Management?</t>
+  </si>
+  <si>
+    <t>Has testing been conducted and the findings logged in Incident Management?</t>
+  </si>
+  <si>
+    <t>Has the Project plan been updated?</t>
+  </si>
+  <si>
+    <t>Have the integration steps been verified? Have the defects been logged in the Incident Management?</t>
+  </si>
+  <si>
+    <t>Have the integration test cases been reviewed and the defects logged in Incident Management?</t>
+  </si>
+  <si>
+    <t>Have the above been reviewed and defecs logged in Incident Management?</t>
+  </si>
+  <si>
+    <t>Has the product been validated and the defects logged in Incident Management?</t>
+  </si>
+  <si>
+    <t>Are the project learnings proposed in Incident learnings, actionable and specific?</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1667,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="31"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="30"/>
-    <tableColumn id="3" name="Major Non-Conformance/ Minor Non-Conformance/ Observation" dataDxfId="29"/>
+    <tableColumn id="3" name="Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation" dataDxfId="29"/>
     <tableColumn id="4" name="Log ID" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1681,12 +1675,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:D63" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="A10:D63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:D62" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="A10:D62"/>
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="24"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="23"/>
-    <tableColumn id="3" name="Major Non-Conformance/ Minor Non-Conformance/ Observation" dataDxfId="22"/>
+    <tableColumn id="3" name="Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation" dataDxfId="22"/>
     <tableColumn id="4" name="Log ID" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1699,7 +1693,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="17"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="16"/>
-    <tableColumn id="3" name="Major Non-Conformance/ Minor Non-Conformance/ Observation" dataDxfId="15"/>
+    <tableColumn id="3" name="Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation" dataDxfId="15"/>
     <tableColumn id="4" name="Log ID" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -1712,7 +1706,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="10"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="9"/>
-    <tableColumn id="3" name="Major Non-Conformance/ Minor Non-Conformance/ Observation" dataDxfId="8"/>
+    <tableColumn id="3" name="Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation" dataDxfId="8"/>
     <tableColumn id="4" name="Log ID" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -1725,7 +1719,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="3"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="2"/>
-    <tableColumn id="3" name="Major Non-Conformance/ Minor Non-Conformance/ Observation" dataDxfId="1"/>
+    <tableColumn id="3" name="Functional Non-Conformance/ Non-Functional Non-Conformance/ Observation" dataDxfId="1"/>
     <tableColumn id="4" name="Log ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -2022,7 +2016,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,17 +2028,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2056,15 +2050,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="61" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.5703125" style="61" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="61" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="61" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="61" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="61"/>
   </cols>
@@ -2076,26 +2070,26 @@
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>0</v>
       </c>
@@ -2103,10 +2097,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>71</v>
+        <v>146</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="65"/>
@@ -2152,7 +2146,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C15" s="65"/>
       <c r="D15" s="65"/>
@@ -2162,7 +2156,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C16" s="65"/>
       <c r="D16" s="65"/>
@@ -2182,7 +2176,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
@@ -2200,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="65"/>
@@ -2210,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="65"/>
@@ -2250,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="65"/>
@@ -2280,7 +2274,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="65"/>
@@ -2308,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="65"/>
@@ -2318,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="65"/>
@@ -2328,7 +2322,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="10"/>
@@ -2338,7 +2332,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="10"/>
@@ -2348,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="10"/>
@@ -2358,7 +2352,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="10"/>
@@ -2368,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="71" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="71"/>
@@ -2378,7 +2372,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="10"/>
@@ -2388,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C39" s="65"/>
       <c r="D39" s="71"/>
@@ -2398,7 +2392,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C40" s="71"/>
       <c r="D40" s="71"/>
@@ -2416,7 +2410,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="72"/>
       <c r="B42" s="73" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C42" s="72"/>
       <c r="D42" s="72"/>
@@ -2426,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -2476,7 +2470,7 @@
         <v>6</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -2496,7 +2490,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -2538,17 +2532,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2560,37 +2554,37 @@
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>71</v>
+      <c r="C10" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2608,7 +2602,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -2628,7 +2622,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -2638,7 +2632,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="37"/>
@@ -2658,7 +2652,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -2668,7 +2662,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
@@ -2678,7 +2672,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="50"/>
@@ -2708,486 +2702,476 @@
         <v>12</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="37"/>
+        <v>100</v>
+      </c>
+      <c r="C24" s="31"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="48">
-        <v>15</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>105</v>
+        <v>16</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>90</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="48">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:4" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="48">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="48">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="48">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>
     </row>
-    <row r="33" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="48">
-        <v>23</v>
-      </c>
-      <c r="B33" s="51" t="s">
-        <v>96</v>
+        <v>24</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
     </row>
-    <row r="34" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
     </row>
     <row r="36" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
     </row>
-    <row r="37" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="48">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
     </row>
-    <row r="39" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="48">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-    </row>
-    <row r="42" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="48">
-        <v>32</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="75"/>
+      <c r="D41" s="75"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
+      <c r="A43" s="48">
+        <v>1</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="31"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="31"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="31"/>
     </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="31"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="31"/>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="31"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="48">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="31"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="48">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="31"/>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="31"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="31"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="31"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="31"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="31"/>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="37"/>
+        <v>150</v>
+      </c>
+      <c r="C61" s="31"/>
       <c r="D61" s="31"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="48">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="48">
-        <v>20</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-    </row>
-    <row r="64" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="38"/>
-      <c r="B64" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="45">
+    <row r="63" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="38"/>
+      <c r="B63" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="45">
         <v>1</v>
       </c>
+      <c r="B64" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="52">
+        <v>2</v>
+      </c>
       <c r="B65" s="44" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37"/>
     </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="52">
-        <v>2</v>
-      </c>
-      <c r="B66" s="44" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>83</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="52">
-        <v>3</v>
-      </c>
-      <c r="B67" s="45" t="s">
-        <v>86</v>
+        <v>4</v>
+      </c>
+      <c r="B67" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37"/>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B68" s="44" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37"/>
-    </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="52">
-        <v>5</v>
-      </c>
-      <c r="B69" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44:C61 C11:C42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43:C60 C11:C41">
       <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D63">
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3203,42 +3187,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="33" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="33" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3249,11 +3233,11 @@
       <c r="B8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>71</v>
+      <c r="C8" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3261,7 +3245,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="37"/>
@@ -3271,7 +3255,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
@@ -3281,7 +3265,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -3291,7 +3275,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -3321,7 +3305,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
@@ -3331,7 +3315,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="37"/>
@@ -3341,7 +3325,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -3351,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
@@ -3361,7 +3345,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
@@ -3371,7 +3355,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
@@ -3381,7 +3365,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
@@ -3391,7 +3375,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
@@ -3401,7 +3385,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
@@ -3411,7 +3395,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
@@ -3421,7 +3405,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -3430,8 +3414,8 @@
       <c r="A26" s="44">
         <v>18</v>
       </c>
-      <c r="B26" s="49" t="s">
-        <v>146</v>
+      <c r="B26" s="44" t="s">
+        <v>151</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
@@ -3441,7 +3425,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -3451,7 +3435,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
@@ -3461,17 +3445,17 @@
         <v>21</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="49">
         <v>22</v>
       </c>
-      <c r="B30" s="49" t="s">
-        <v>148</v>
+      <c r="B30" s="44" t="s">
+        <v>152</v>
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
@@ -3481,7 +3465,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
@@ -3491,7 +3475,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -3519,7 +3503,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
@@ -3539,7 +3523,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
@@ -3549,7 +3533,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
@@ -3559,7 +3543,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
@@ -3569,7 +3553,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="37"/>
@@ -3579,7 +3563,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="49"/>
@@ -3589,7 +3573,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -3599,7 +3583,7 @@
         <v>13</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C43" s="49"/>
       <c r="D43" s="49"/>
@@ -3609,7 +3593,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C44" s="49"/>
       <c r="D44" s="49"/>
@@ -3619,7 +3603,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C45" s="56"/>
       <c r="D45" s="56"/>
@@ -3629,7 +3613,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C46" s="44"/>
       <c r="D46" s="44"/>
@@ -3639,7 +3623,7 @@
         <v>17</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47" s="46"/>
       <c r="D47" s="46"/>
@@ -3649,7 +3633,7 @@
         <v>18</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C48" s="46"/>
       <c r="D48" s="46"/>
@@ -3659,7 +3643,7 @@
         <v>19</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C49" s="49"/>
       <c r="D49" s="49"/>
@@ -3668,8 +3652,8 @@
       <c r="A50" s="57">
         <v>20</v>
       </c>
-      <c r="B50" s="49" t="s">
-        <v>120</v>
+      <c r="B50" s="44" t="s">
+        <v>150</v>
       </c>
       <c r="C50" s="49"/>
       <c r="D50" s="49"/>
@@ -3678,8 +3662,8 @@
       <c r="A51" s="57">
         <v>21</v>
       </c>
-      <c r="B51" s="49" t="s">
-        <v>122</v>
+      <c r="B51" s="44" t="s">
+        <v>145</v>
       </c>
       <c r="C51" s="49"/>
       <c r="D51" s="49"/>
@@ -3692,12 +3676,12 @@
       <c r="C52" s="42"/>
       <c r="D52" s="42"/>
     </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="56">
         <v>1</v>
       </c>
-      <c r="B53" s="56" t="s">
-        <v>40</v>
+      <c r="B53" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="37"/>
@@ -3707,7 +3691,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="37"/>
@@ -3717,7 +3701,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="37"/>
@@ -3757,7 +3741,7 @@
         <v>7</v>
       </c>
       <c r="B59" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37"/>
@@ -3765,7 +3749,7 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="38"/>
       <c r="B60" s="39" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
@@ -3775,7 +3759,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37"/>
@@ -3795,7 +3779,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="44" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C63" s="49"/>
       <c r="D63" s="49"/>
@@ -3825,7 +3809,7 @@
         <v>6</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="56"/>
@@ -3835,7 +3819,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="56"/>
@@ -3861,57 +3845,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="33" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>71</v>
+      <c r="C9" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3919,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
@@ -3929,7 +3913,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -3939,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -3949,17 +3933,17 @@
         <v>4</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>5</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -3969,7 +3953,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="49"/>
@@ -3979,7 +3963,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="49"/>
@@ -4009,7 +3993,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4057,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
@@ -4067,7 +4051,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -4077,7 +4061,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
@@ -4087,7 +4071,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="37"/>
@@ -4097,7 +4081,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
@@ -4107,7 +4091,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
@@ -4117,7 +4101,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
@@ -4127,7 +4111,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
@@ -4137,7 +4121,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -4147,7 +4131,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C33" s="49"/>
       <c r="D33" s="56"/>
@@ -4157,7 +4141,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="44"/>
@@ -4167,7 +4151,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C35" s="49"/>
       <c r="D35" s="46"/>
@@ -4177,7 +4161,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C36" s="49"/>
       <c r="D36" s="46"/>
@@ -4187,7 +4171,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C37" s="49"/>
       <c r="D37" s="49"/>
@@ -4196,8 +4180,8 @@
       <c r="A38" s="48">
         <v>18</v>
       </c>
-      <c r="B38" s="49" t="s">
-        <v>120</v>
+      <c r="B38" s="44" t="s">
+        <v>150</v>
       </c>
       <c r="C38" s="49"/>
       <c r="D38" s="49"/>
@@ -4207,7 +4191,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C39" s="49"/>
       <c r="D39" s="37"/>
@@ -4225,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="37"/>
@@ -4235,7 +4219,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="37"/>
@@ -4265,7 +4249,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C45" s="49"/>
       <c r="D45" s="37"/>
@@ -4275,7 +4259,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="49"/>
       <c r="D46" s="37"/>
@@ -4283,7 +4267,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="39" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C47" s="38"/>
       <c r="D47" s="38"/>
@@ -4303,7 +4287,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C49" s="49"/>
       <c r="D49" s="49"/>
@@ -4323,7 +4307,7 @@
         <v>4</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="49"/>
       <c r="D51" s="49"/>
@@ -4358,15 +4342,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4377,22 +4361,22 @@
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -4404,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>71</v>
+        <v>146</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4415,7 +4399,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -4425,17 +4409,17 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -4445,7 +4429,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -4455,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -4485,17 +4469,17 @@
         <v>8</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -4505,7 +4489,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -4515,7 +4499,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -4525,7 +4509,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -4535,7 +4519,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4543,7 +4527,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -4553,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -4563,7 +4547,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -4573,7 +4557,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
@@ -4583,7 +4567,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -4593,7 +4577,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -4621,7 +4605,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -4641,7 +4625,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -4651,7 +4635,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -4661,7 +4645,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -4671,7 +4655,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -4681,7 +4665,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -4691,7 +4675,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -4701,7 +4685,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -4711,7 +4695,7 @@
         <v>11</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -4721,7 +4705,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -4731,7 +4715,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -4741,7 +4725,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -4751,7 +4735,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -4761,7 +4745,7 @@
         <v>16</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -4770,8 +4754,8 @@
       <c r="A45" s="8">
         <v>17</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>120</v>
+      <c r="B45" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -4780,8 +4764,8 @@
       <c r="A46" s="8">
         <v>18</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>122</v>
+      <c r="B46" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -4799,7 +4783,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -4809,7 +4793,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -4849,7 +4833,7 @@
         <v>6</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -4857,7 +4841,7 @@
     <row r="54" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="B54" s="39" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
@@ -4877,7 +4861,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="7"/>
@@ -4887,7 +4871,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="7"/>
@@ -4907,7 +4891,7 @@
         <v>5</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C59" s="12"/>
       <c r="D59" s="7"/>
@@ -4927,7 +4911,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="5"/>
@@ -4950,21 +4934,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -5013,10 +4982,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5036,16 +5027,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Major and Minor words replaced
 by Functional & Non-Functional respectively
</commit_message>
<xml_diff>
--- a/Support/Quality Assurance/CHKL_AUDITT.xlsx
+++ b/Support/Quality Assurance/CHKL_AUDITT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="15240" windowHeight="7995"/>
@@ -447,9 +447,6 @@
     <t>Has  the defects analysis done?</t>
   </si>
   <si>
-    <t>Template Version - 5</t>
-  </si>
-  <si>
     <t>Have the review findings been logged in the Incident Management?</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>Are the project learnings proposed in Incident learnings, actionable and specific?</t>
+  </si>
+  <si>
+    <t>Template Version - 6</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -875,6 +875,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -2016,7 +2017,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,7 +2039,7 @@
     </row>
     <row r="5" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2050,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2097,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="65" t="s">
         <v>69</v>
@@ -2244,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="65"/>
@@ -2274,7 +2275,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="65"/>
@@ -2392,9 +2393,9 @@
         <v>11</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="71"/>
+        <v>144</v>
+      </c>
+      <c r="C40" s="65"/>
       <c r="D40" s="71"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,7 +2405,7 @@
       <c r="B41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,7 +2423,7 @@
       <c r="B43" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2432,7 +2433,7 @@
       <c r="B44" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2442,7 +2443,7 @@
       <c r="B45" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="10"/>
+      <c r="C45" s="77"/>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2452,7 +2453,7 @@
       <c r="B46" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="10"/>
+      <c r="C46" s="77"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2462,7 +2463,7 @@
       <c r="B47" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="10"/>
+      <c r="C47" s="77"/>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2472,7 +2473,7 @@
       <c r="B48" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,7 +2483,7 @@
       <c r="B49" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2492,7 +2493,7 @@
       <c r="B50" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="10"/>
+      <c r="C50" s="77"/>
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,8 +2519,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D11 D19 D42">
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C28 C30:C39">
-      <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C28 C30:C41 C43:C50">
+      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2534,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +2582,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>69</v>
@@ -2594,7 +2595,7 @@
       <c r="B11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,7 +2605,7 @@
       <c r="B12" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2614,7 +2615,7 @@
       <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2624,7 +2625,7 @@
       <c r="B14" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,7 +2635,7 @@
       <c r="B15" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2644,7 +2645,7 @@
       <c r="B16" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,7 +2655,7 @@
       <c r="B17" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2664,7 +2665,7 @@
       <c r="B18" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2674,7 +2675,7 @@
       <c r="B19" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="37"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="50"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2684,7 +2685,7 @@
       <c r="B20" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2694,7 +2695,7 @@
       <c r="B21" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2702,9 +2703,9 @@
         <v>12</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" s="37"/>
+        <v>146</v>
+      </c>
+      <c r="C22" s="77"/>
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,7 +2715,7 @@
       <c r="B23" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2724,7 +2725,7 @@
       <c r="B24" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="31"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2734,7 +2735,7 @@
       <c r="B25" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2744,7 +2745,7 @@
       <c r="B26" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="31"/>
+      <c r="C26" s="77"/>
       <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2754,7 +2755,7 @@
       <c r="B27" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="77"/>
       <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2764,7 +2765,7 @@
       <c r="B28" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="31"/>
+      <c r="C28" s="77"/>
       <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2774,7 +2775,7 @@
       <c r="B29" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="31"/>
+      <c r="C29" s="77"/>
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2784,7 +2785,7 @@
       <c r="B30" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="31"/>
+      <c r="C30" s="77"/>
       <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2792,9 +2793,9 @@
         <v>22</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="C31" s="31"/>
+        <v>147</v>
+      </c>
+      <c r="C31" s="77"/>
       <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2804,7 +2805,7 @@
       <c r="B32" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="31"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2814,7 +2815,7 @@
       <c r="B33" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="31"/>
     </row>
     <row r="34" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2824,7 +2825,7 @@
       <c r="B34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="31"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="31"/>
     </row>
     <row r="35" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2834,7 +2835,7 @@
       <c r="B35" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="31"/>
     </row>
     <row r="36" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2844,7 +2845,7 @@
       <c r="B36" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="31"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="31"/>
     </row>
     <row r="37" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2854,7 +2855,7 @@
       <c r="B37" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2864,7 +2865,7 @@
       <c r="B38" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="31"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="31"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2874,7 +2875,7 @@
       <c r="B39" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="31"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2884,7 +2885,7 @@
       <c r="B40" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="31"/>
+      <c r="C40" s="77"/>
       <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2894,7 +2895,7 @@
       <c r="B41" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="31"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="75"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,7 +2913,7 @@
       <c r="B43" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="37"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="31"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2922,7 +2923,7 @@
       <c r="B44" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="37"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="31"/>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2930,9 +2931,9 @@
         <v>3</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="37"/>
+        <v>148</v>
+      </c>
+      <c r="C45" s="77"/>
       <c r="D45" s="31"/>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2942,7 +2943,7 @@
       <c r="B46" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="37"/>
+      <c r="C46" s="77"/>
       <c r="D46" s="31"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2952,7 +2953,7 @@
       <c r="B47" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="37"/>
+      <c r="C47" s="77"/>
       <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2962,7 +2963,7 @@
       <c r="B48" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="37"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="31"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2972,7 +2973,7 @@
       <c r="B49" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="37"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="31"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2982,7 +2983,7 @@
       <c r="B50" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="37"/>
+      <c r="C50" s="77"/>
       <c r="D50" s="31"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2992,7 +2993,7 @@
       <c r="B51" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="37"/>
+      <c r="C51" s="77"/>
       <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,7 +3003,7 @@
       <c r="B52" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="37"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="31"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,7 +3013,7 @@
       <c r="B53" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="37"/>
+      <c r="C53" s="77"/>
       <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3022,7 +3023,7 @@
       <c r="B54" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="37"/>
+      <c r="C54" s="77"/>
       <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3032,7 +3033,7 @@
       <c r="B55" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="37"/>
+      <c r="C55" s="77"/>
       <c r="D55" s="31"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3042,7 +3043,7 @@
       <c r="B56" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="37"/>
+      <c r="C56" s="77"/>
       <c r="D56" s="31"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,7 +3053,7 @@
       <c r="B57" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="37"/>
+      <c r="C57" s="77"/>
       <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3062,7 +3063,7 @@
       <c r="B58" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="37"/>
+      <c r="C58" s="77"/>
       <c r="D58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,7 +3073,7 @@
       <c r="B59" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="37"/>
+      <c r="C59" s="77"/>
       <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3082,7 +3083,7 @@
       <c r="B60" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="37"/>
+      <c r="C60" s="77"/>
       <c r="D60" s="31"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3090,9 +3091,9 @@
         <v>19</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="C61" s="31"/>
+        <v>149</v>
+      </c>
+      <c r="C61" s="77"/>
       <c r="D61" s="31"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3100,9 +3101,9 @@
         <v>20</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="31"/>
+        <v>144</v>
+      </c>
+      <c r="C62" s="77"/>
       <c r="D62" s="31"/>
     </row>
     <row r="63" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3120,7 +3121,7 @@
       <c r="B64" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="37"/>
+      <c r="C64" s="77"/>
       <c r="D64" s="37"/>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3130,7 +3131,7 @@
       <c r="B65" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="C65" s="37"/>
+      <c r="C65" s="77"/>
       <c r="D65" s="37"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3140,7 +3141,7 @@
       <c r="B66" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C66" s="37"/>
+      <c r="C66" s="77"/>
       <c r="D66" s="37"/>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3150,7 +3151,7 @@
       <c r="B67" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="37"/>
+      <c r="C67" s="77"/>
       <c r="D67" s="37"/>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3160,7 +3161,7 @@
       <c r="B68" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="37"/>
+      <c r="C68" s="77"/>
       <c r="D68" s="37"/>
     </row>
   </sheetData>
@@ -3168,11 +3169,11 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43:C60 C11:C41">
-      <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D63">
       <formula1>"Major, Minor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C41 C43:C62 C64:C68">
+      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3187,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" s="37" t="s">
         <v>69</v>
@@ -3247,7 +3248,7 @@
       <c r="B9" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="37"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,7 +3258,7 @@
       <c r="B10" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="37"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3267,7 +3268,7 @@
       <c r="B11" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3277,7 +3278,7 @@
       <c r="B12" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,7 +3288,7 @@
       <c r="B13" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3297,7 +3298,7 @@
       <c r="B14" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3307,7 +3308,7 @@
       <c r="B15" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3317,7 +3318,7 @@
       <c r="B16" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3327,7 +3328,7 @@
       <c r="B17" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3337,7 +3338,7 @@
       <c r="B18" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3345,9 +3346,9 @@
         <v>11</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="37"/>
+        <v>150</v>
+      </c>
+      <c r="C19" s="77"/>
       <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3357,7 +3358,7 @@
       <c r="B20" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3367,7 +3368,7 @@
       <c r="B21" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3377,7 +3378,7 @@
       <c r="B22" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="37"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3387,7 +3388,7 @@
       <c r="B23" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3397,7 +3398,7 @@
       <c r="B24" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3407,7 +3408,7 @@
       <c r="B25" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3415,9 +3416,9 @@
         <v>18</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="37"/>
+        <v>150</v>
+      </c>
+      <c r="C26" s="77"/>
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3427,7 +3428,7 @@
       <c r="B27" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="77"/>
       <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3437,7 +3438,7 @@
       <c r="B28" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="77"/>
       <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3447,7 +3448,7 @@
       <c r="B29" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="77"/>
       <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3455,9 +3456,9 @@
         <v>22</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="49"/>
+        <v>151</v>
+      </c>
+      <c r="C30" s="77"/>
       <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3467,7 +3468,7 @@
       <c r="B31" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="77"/>
       <c r="D31" s="49"/>
     </row>
     <row r="32" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3477,7 +3478,7 @@
       <c r="B32" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3495,7 +3496,7 @@
       <c r="B34" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="37"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="37"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3505,7 +3506,7 @@
       <c r="B35" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="37"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="37"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3515,7 +3516,7 @@
       <c r="B36" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="37"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="37"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3525,7 +3526,7 @@
       <c r="B37" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="C37" s="37"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="37"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3535,7 +3536,7 @@
       <c r="B38" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="37"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="37"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3545,7 +3546,7 @@
       <c r="B39" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="37"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,9 +3554,9 @@
         <v>8</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="37"/>
+        <v>152</v>
+      </c>
+      <c r="C40" s="77"/>
       <c r="D40" s="37"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3565,7 +3566,7 @@
       <c r="B41" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="49"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3575,7 +3576,7 @@
       <c r="B42" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="49"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,7 +3586,7 @@
       <c r="B43" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="49"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="49"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3595,7 +3596,7 @@
       <c r="B44" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="49"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3605,7 +3606,7 @@
       <c r="B45" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="56"/>
+      <c r="C45" s="77"/>
       <c r="D45" s="56"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3616,7 @@
       <c r="B46" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="44"/>
+      <c r="C46" s="77"/>
       <c r="D46" s="44"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,7 +3626,7 @@
       <c r="B47" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="46"/>
+      <c r="C47" s="77"/>
       <c r="D47" s="46"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3635,7 +3636,7 @@
       <c r="B48" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="46"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="46"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3645,7 +3646,7 @@
       <c r="B49" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="49"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="49"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,9 +3654,9 @@
         <v>20</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C50" s="49"/>
+        <v>149</v>
+      </c>
+      <c r="C50" s="77"/>
       <c r="D50" s="49"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,9 +3664,9 @@
         <v>21</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="49"/>
+        <v>144</v>
+      </c>
+      <c r="C51" s="77"/>
       <c r="D51" s="49"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3683,7 +3684,7 @@
       <c r="B53" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="37"/>
+      <c r="C53" s="77"/>
       <c r="D53" s="37"/>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3693,7 +3694,7 @@
       <c r="B54" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="37"/>
+      <c r="C54" s="77"/>
       <c r="D54" s="37"/>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3703,7 +3704,7 @@
       <c r="B55" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C55" s="37"/>
+      <c r="C55" s="77"/>
       <c r="D55" s="37"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3713,7 +3714,7 @@
       <c r="B56" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="37"/>
+      <c r="C56" s="77"/>
       <c r="D56" s="37"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3723,7 +3724,7 @@
       <c r="B57" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="37"/>
+      <c r="C57" s="77"/>
       <c r="D57" s="37"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,7 +3734,7 @@
       <c r="B58" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C58" s="37"/>
+      <c r="C58" s="77"/>
       <c r="D58" s="37"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3743,7 +3744,7 @@
       <c r="B59" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="37"/>
+      <c r="C59" s="77"/>
       <c r="D59" s="37"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,7 +3762,7 @@
       <c r="B61" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="37"/>
+      <c r="C61" s="77"/>
       <c r="D61" s="37"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3771,7 +3772,7 @@
       <c r="B62" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="37"/>
+      <c r="C62" s="77"/>
       <c r="D62" s="49"/>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3781,7 +3782,7 @@
       <c r="B63" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="49"/>
+      <c r="C63" s="77"/>
       <c r="D63" s="49"/>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3791,7 +3792,7 @@
       <c r="B64" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="49"/>
+      <c r="C64" s="77"/>
       <c r="D64" s="49"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3801,7 +3802,7 @@
       <c r="B65" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="49"/>
+      <c r="C65" s="77"/>
       <c r="D65" s="49"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,7 +3812,7 @@
       <c r="B66" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="C66" s="37"/>
+      <c r="C66" s="77"/>
       <c r="D66" s="56"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,16 +3822,16 @@
       <c r="B67" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="37"/>
+      <c r="C67" s="77"/>
       <c r="D67" s="56"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53:C59 C61:C67 C34:C51 C9:C32">
-      <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D60">
       <formula1>"Major, Minor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C32 C34:C51 C53:C59 C61:C67">
+      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3845,8 +3846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3892,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" s="37" t="s">
         <v>69</v>
@@ -3903,9 +3904,9 @@
         <v>1</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="37"/>
+        <v>153</v>
+      </c>
+      <c r="C10" s="77"/>
       <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3915,7 +3916,7 @@
       <c r="B11" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3925,7 +3926,7 @@
       <c r="B12" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,7 +3936,7 @@
       <c r="B13" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3943,9 +3944,9 @@
         <v>5</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="37"/>
+        <v>154</v>
+      </c>
+      <c r="C14" s="77"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,7 +3956,7 @@
       <c r="B15" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3965,7 +3966,7 @@
       <c r="B16" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,7 +3976,7 @@
       <c r="B17" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,7 +3986,7 @@
       <c r="B18" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3995,7 +3996,7 @@
       <c r="B19" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4013,7 +4014,7 @@
       <c r="B21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4023,7 +4024,7 @@
       <c r="B22" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="37"/>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4033,7 +4034,7 @@
       <c r="B23" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4043,7 +4044,7 @@
       <c r="B24" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4053,7 +4054,7 @@
       <c r="B25" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4063,7 +4064,7 @@
       <c r="B26" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="37"/>
+      <c r="C26" s="77"/>
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4073,7 +4074,7 @@
       <c r="B27" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="37"/>
+      <c r="C27" s="77"/>
       <c r="D27" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,7 +4084,7 @@
       <c r="B28" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="77"/>
       <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,7 +4094,7 @@
       <c r="B29" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="77"/>
       <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4103,7 +4104,7 @@
       <c r="B30" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="49"/>
+      <c r="C30" s="77"/>
       <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4114,7 @@
       <c r="B31" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="77"/>
       <c r="D31" s="49"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4123,7 +4124,7 @@
       <c r="B32" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="49"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="49"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,7 +4134,7 @@
       <c r="B33" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="49"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="56"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4143,7 +4144,7 @@
       <c r="B34" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="49"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="44"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,7 +4154,7 @@
       <c r="B35" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="49"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="46"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4163,7 +4164,7 @@
       <c r="B36" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="46"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4173,7 +4174,7 @@
       <c r="B37" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="49"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="49"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,9 +4182,9 @@
         <v>18</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="49"/>
+        <v>149</v>
+      </c>
+      <c r="C38" s="77"/>
       <c r="D38" s="49"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4191,9 +4192,9 @@
         <v>19</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="C39" s="49"/>
+        <v>144</v>
+      </c>
+      <c r="C39" s="77"/>
       <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,7 +4212,7 @@
       <c r="B41" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="37"/>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4221,7 +4222,7 @@
       <c r="B42" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,7 +4232,7 @@
       <c r="B43" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="49"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="37"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4241,7 +4242,7 @@
       <c r="B44" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="37"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4252,7 @@
       <c r="B45" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="49"/>
+      <c r="C45" s="77"/>
       <c r="D45" s="37"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,7 +4262,7 @@
       <c r="B46" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="49"/>
+      <c r="C46" s="77"/>
       <c r="D46" s="37"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4279,7 +4280,7 @@
       <c r="B48" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="49"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="49"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4289,7 +4290,7 @@
       <c r="B49" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="49"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="49"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4299,7 +4300,7 @@
       <c r="B50" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="49"/>
+      <c r="C50" s="77"/>
       <c r="D50" s="49"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4309,7 +4310,7 @@
       <c r="B51" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="49"/>
+      <c r="C51" s="77"/>
       <c r="D51" s="49"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4319,16 +4320,16 @@
       <c r="B52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="49"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C41:C46 C48:C52 C21:C39 C10:C19">
-      <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D47">
       <formula1>"Major, Minor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C19 C21:C39 C41:C46 C48:C52">
+      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4343,7 +4344,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="C55" sqref="C55:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>69</v>
@@ -4401,7 +4402,7 @@
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4411,7 +4412,7 @@
       <c r="B10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4419,9 +4420,9 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="C11" s="77"/>
       <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4432,7 @@
       <c r="B12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4441,7 +4442,7 @@
       <c r="B13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4451,7 +4452,7 @@
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4462,7 @@
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4471,7 +4472,7 @@
       <c r="B16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4479,9 +4480,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="C17" s="77"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4492,7 @@
       <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4501,7 +4502,7 @@
       <c r="B19" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4511,7 +4512,7 @@
       <c r="B20" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4521,7 +4522,7 @@
       <c r="B21" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4539,7 +4540,7 @@
       <c r="B23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4549,7 +4550,7 @@
       <c r="B24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,7 +4560,7 @@
       <c r="B25" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4567,9 +4568,9 @@
         <v>4</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>157</v>
+      </c>
+      <c r="C26" s="77"/>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4579,7 +4580,7 @@
       <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="77"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4597,7 +4598,7 @@
       <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="77"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4607,7 +4608,7 @@
       <c r="B30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="77"/>
       <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4617,7 +4618,7 @@
       <c r="B31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="77"/>
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4627,7 +4628,7 @@
       <c r="B32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4637,7 +4638,7 @@
       <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4647,7 +4648,7 @@
       <c r="B34" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4655,9 +4656,9 @@
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="12"/>
+        <v>152</v>
+      </c>
+      <c r="C35" s="77"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4667,7 +4668,7 @@
       <c r="B36" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4677,7 +4678,7 @@
       <c r="B37" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4687,7 +4688,7 @@
       <c r="B38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4697,7 +4698,7 @@
       <c r="B39" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4707,7 +4708,7 @@
       <c r="B40" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="77"/>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4717,7 +4718,7 @@
       <c r="B41" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4727,7 +4728,7 @@
       <c r="B42" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4737,7 +4738,7 @@
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="19"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:4" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4747,7 +4748,7 @@
       <c r="B44" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4755,9 +4756,9 @@
         <v>17</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" s="7"/>
+        <v>149</v>
+      </c>
+      <c r="C45" s="77"/>
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4765,9 +4766,9 @@
         <v>18</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="7"/>
+        <v>144</v>
+      </c>
+      <c r="C46" s="77"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,7 +4786,7 @@
       <c r="B48" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4795,7 +4796,7 @@
       <c r="B49" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,7 +4806,7 @@
       <c r="B50" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="12"/>
+      <c r="C50" s="77"/>
       <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4815,7 +4816,7 @@
       <c r="B51" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="77"/>
       <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,7 +4826,7 @@
       <c r="B52" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,7 +4836,7 @@
       <c r="B53" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="12"/>
+      <c r="C53" s="77"/>
       <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -4853,7 +4854,7 @@
       <c r="B55" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="12"/>
+      <c r="C55" s="77"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4863,7 +4864,7 @@
       <c r="B56" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C56" s="12"/>
+      <c r="C56" s="77"/>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4873,7 +4874,7 @@
       <c r="B57" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="77"/>
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4883,7 +4884,7 @@
       <c r="B58" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="12"/>
+      <c r="C58" s="77"/>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4893,7 +4894,7 @@
       <c r="B59" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="12"/>
+      <c r="C59" s="77"/>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4903,7 +4904,7 @@
       <c r="B60" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="77"/>
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4913,7 +4914,7 @@
       <c r="B61" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C61" s="12"/>
+      <c r="C61" s="77"/>
       <c r="D61" s="5"/>
     </row>
   </sheetData>
@@ -4921,8 +4922,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D47 D28 D54 A28">
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44:C46 C23:C27 C9:C21 C29:C35 C48:C53 C55:C61">
-      <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C21 C23:C27 C29:C46 C48:C53 C55:C61">
+      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4934,6 +4935,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -4982,32 +4998,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5027,9 +5021,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Assets, knowledge & technology
identification points added in planning phase list.
</commit_message>
<xml_diff>
--- a/Support/Quality Assurance/CHKL_AUDITT.xlsx
+++ b/Support/Quality Assurance/CHKL_AUDITT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="161">
   <si>
     <t>S. No</t>
   </si>
@@ -114,12 +114,6 @@
     <t>Have the requirements been reviewed using Requirement Review Checklist?</t>
   </si>
   <si>
-    <t>Has the project plan been established using as per the defined and current Project Plan template?</t>
-  </si>
-  <si>
-    <t>Has the Risk management plan been prepared for identification and mitigation of project risks?</t>
-  </si>
-  <si>
     <t>Has the Plan review checklist been used for the review and the same archived? Verify the plan with respect to the populated review checklist on a sampling basis.</t>
   </si>
   <si>
@@ -496,6 +490,18 @@
   </si>
   <si>
     <t>Template Version - 6</t>
+  </si>
+  <si>
+    <t>Has the project plan been established using as per the defined and current on GIL.ef &amp; Project Plan template?</t>
+  </si>
+  <si>
+    <t>Has the Risk management plan been prepared for identification and mitigation of project risks and identification &amp; leverage of Project Opportunities?</t>
+  </si>
+  <si>
+    <t>Has the Project's Financials identified clearly?</t>
+  </si>
+  <si>
+    <t>Has the Project's Assests, Knowledge &amp; Technology identified clearly?</t>
   </si>
 </sst>
 </file>
@@ -583,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -674,6 +680,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -681,7 +700,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -872,10 +891,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -1676,8 +1698,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:D62" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="A10:D62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:D64" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="A10:D64"/>
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="24"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="23"/>
@@ -2016,9 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2029,17 +2049,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2051,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,22 +2091,22 @@
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2098,10 +2118,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,7 +2139,7 @@
       <c r="B12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="65"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2129,7 +2149,7 @@
       <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="65"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2137,9 +2157,9 @@
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="65"/>
+        <v>114</v>
+      </c>
+      <c r="C14" s="76"/>
       <c r="D14" s="65"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2147,9 +2167,9 @@
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="65"/>
+        <v>115</v>
+      </c>
+      <c r="C15" s="76"/>
       <c r="D15" s="65"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2157,9 +2177,9 @@
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="65"/>
+        <v>117</v>
+      </c>
+      <c r="C16" s="76"/>
       <c r="D16" s="65"/>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2169,7 +2189,7 @@
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="65"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="65"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,9 +2197,9 @@
         <v>7</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="65"/>
+        <v>87</v>
+      </c>
+      <c r="C18" s="76"/>
       <c r="D18" s="65"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,9 +2215,9 @@
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="65"/>
+        <v>118</v>
+      </c>
+      <c r="C20" s="76"/>
       <c r="D20" s="65"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2205,9 +2225,9 @@
         <v>2</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="65"/>
+        <v>119</v>
+      </c>
+      <c r="C21" s="76"/>
       <c r="D21" s="65"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2217,7 +2237,7 @@
       <c r="B22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="65"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="65"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,7 +2247,7 @@
       <c r="B23" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="65"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="65"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2237,7 +2257,7 @@
       <c r="B24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="65"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="65"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2245,9 +2265,9 @@
         <v>6</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C25" s="65"/>
+        <v>140</v>
+      </c>
+      <c r="C25" s="76"/>
       <c r="D25" s="65"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,7 +2277,7 @@
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="65"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="65"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,7 +2287,7 @@
       <c r="B27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="65"/>
+      <c r="C27" s="76"/>
       <c r="D27" s="65"/>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2275,9 +2295,9 @@
         <v>9</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="65"/>
+        <v>141</v>
+      </c>
+      <c r="C28" s="76"/>
       <c r="D28" s="65"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2295,7 +2315,7 @@
       <c r="B30" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="65"/>
+      <c r="C30" s="76"/>
       <c r="D30" s="65"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2303,9 +2323,9 @@
         <v>2</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="65"/>
+        <v>128</v>
+      </c>
+      <c r="C31" s="76"/>
       <c r="D31" s="65"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2313,9 +2333,9 @@
         <v>3</v>
       </c>
       <c r="B32" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="65"/>
+        <v>64</v>
+      </c>
+      <c r="C32" s="76"/>
       <c r="D32" s="65"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2323,9 +2343,9 @@
         <v>4</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="65"/>
+        <v>68</v>
+      </c>
+      <c r="C33" s="76"/>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2333,9 +2353,9 @@
         <v>5</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="65"/>
+        <v>69</v>
+      </c>
+      <c r="C34" s="76"/>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2343,9 +2363,9 @@
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="65"/>
+        <v>70</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2353,9 +2373,9 @@
         <v>7</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="65"/>
+        <v>71</v>
+      </c>
+      <c r="C36" s="76"/>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2363,9 +2383,9 @@
         <v>8</v>
       </c>
       <c r="B37" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="65"/>
+        <v>72</v>
+      </c>
+      <c r="C37" s="76"/>
       <c r="D37" s="71"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2373,9 +2393,9 @@
         <v>9</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="65"/>
+        <v>74</v>
+      </c>
+      <c r="C38" s="76"/>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2383,9 +2403,9 @@
         <v>10</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="65"/>
+        <v>75</v>
+      </c>
+      <c r="C39" s="76"/>
       <c r="D39" s="71"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2393,9 +2413,9 @@
         <v>11</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" s="65"/>
+        <v>142</v>
+      </c>
+      <c r="C40" s="76"/>
       <c r="D40" s="71"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2405,13 +2425,13 @@
       <c r="B41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="65"/>
+      <c r="C41" s="76"/>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="72"/>
       <c r="B42" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" s="72"/>
       <c r="D42" s="72"/>
@@ -2421,9 +2441,9 @@
         <v>1</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="77"/>
+        <v>116</v>
+      </c>
+      <c r="C43" s="76"/>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2433,7 +2453,7 @@
       <c r="B44" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="76"/>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2443,7 +2463,7 @@
       <c r="B45" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="77"/>
+      <c r="C45" s="76"/>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2453,7 +2473,7 @@
       <c r="B46" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="77"/>
+      <c r="C46" s="76"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2463,7 +2483,7 @@
       <c r="B47" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="77"/>
+      <c r="C47" s="76"/>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2471,9 +2491,9 @@
         <v>6</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="77"/>
+        <v>120</v>
+      </c>
+      <c r="C48" s="76"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,7 +2503,7 @@
       <c r="B49" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="77"/>
+      <c r="C49" s="76"/>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2491,9 +2511,9 @@
         <v>8</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50" s="77"/>
+        <v>76</v>
+      </c>
+      <c r="C50" s="76"/>
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,7 +2540,7 @@
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C28 C30:C41 C43:C50">
-      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2533,10 +2553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,29 +2568,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="77"/>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2582,10 +2602,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2593,9 +2613,9 @@
         <v>1</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="77"/>
+        <v>157</v>
+      </c>
+      <c r="C11" s="76"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2603,19 +2623,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="77"/>
+        <v>64</v>
+      </c>
+      <c r="C12" s="76"/>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>3</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="77"/>
+        <v>158</v>
+      </c>
+      <c r="C13" s="76"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2623,9 +2643,9 @@
         <v>4</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="77"/>
+        <v>97</v>
+      </c>
+      <c r="C14" s="76"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,9 +2653,9 @@
         <v>5</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="77"/>
+        <v>66</v>
+      </c>
+      <c r="C15" s="76"/>
       <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2643,9 +2663,9 @@
         <v>6</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="77"/>
+        <v>32</v>
+      </c>
+      <c r="C16" s="76"/>
       <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2653,9 +2673,9 @@
         <v>7</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="77"/>
+        <v>59</v>
+      </c>
+      <c r="C17" s="76"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2663,9 +2683,9 @@
         <v>8</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="77"/>
+        <v>60</v>
+      </c>
+      <c r="C18" s="76"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2673,9 +2693,9 @@
         <v>9</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="77"/>
+        <v>122</v>
+      </c>
+      <c r="C19" s="76"/>
       <c r="D19" s="50"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2685,7 +2705,7 @@
       <c r="B20" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="77"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2693,9 +2713,9 @@
         <v>11</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="77"/>
+        <v>31</v>
+      </c>
+      <c r="C21" s="76"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2703,9 +2723,9 @@
         <v>12</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="77"/>
+        <v>144</v>
+      </c>
+      <c r="C22" s="76"/>
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,9 +2733,9 @@
         <v>14</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="77"/>
+        <v>33</v>
+      </c>
+      <c r="C23" s="76"/>
       <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2723,9 +2743,9 @@
         <v>15</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="77"/>
+        <v>98</v>
+      </c>
+      <c r="C24" s="76"/>
       <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2733,9 +2753,9 @@
         <v>16</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="77"/>
+        <v>88</v>
+      </c>
+      <c r="C25" s="76"/>
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2743,9 +2763,9 @@
         <v>17</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="77"/>
+        <v>123</v>
+      </c>
+      <c r="C26" s="76"/>
       <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2753,9 +2773,9 @@
         <v>18</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="77"/>
+        <v>87</v>
+      </c>
+      <c r="C27" s="76"/>
       <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2763,9 +2783,9 @@
         <v>19</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="77"/>
+        <v>89</v>
+      </c>
+      <c r="C28" s="76"/>
       <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2773,9 +2793,9 @@
         <v>20</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="77"/>
+        <v>99</v>
+      </c>
+      <c r="C29" s="76"/>
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2783,9 +2803,9 @@
         <v>21</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="77"/>
+        <v>100</v>
+      </c>
+      <c r="C30" s="76"/>
       <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2793,9 +2813,9 @@
         <v>22</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="77"/>
+        <v>145</v>
+      </c>
+      <c r="C31" s="76"/>
       <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:4" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2803,9 +2823,9 @@
         <v>23</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="77"/>
+        <v>90</v>
+      </c>
+      <c r="C32" s="76"/>
       <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2813,9 +2833,9 @@
         <v>24</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="77"/>
+        <v>73</v>
+      </c>
+      <c r="C33" s="76"/>
       <c r="D33" s="31"/>
     </row>
     <row r="34" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,9 +2843,9 @@
         <v>25</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="77"/>
+        <v>82</v>
+      </c>
+      <c r="C34" s="76"/>
       <c r="D34" s="31"/>
     </row>
     <row r="35" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2833,9 +2853,9 @@
         <v>26</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="77"/>
+        <v>92</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="31"/>
     </row>
     <row r="36" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2843,9 +2863,9 @@
         <v>27</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="77"/>
+        <v>93</v>
+      </c>
+      <c r="C36" s="76"/>
       <c r="D36" s="31"/>
     </row>
     <row r="37" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2853,9 +2873,9 @@
         <v>28</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="77"/>
+        <v>94</v>
+      </c>
+      <c r="C37" s="76"/>
       <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2863,9 +2883,9 @@
         <v>29</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="77"/>
+        <v>95</v>
+      </c>
+      <c r="C38" s="76"/>
       <c r="D38" s="31"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2873,9 +2893,9 @@
         <v>30</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="77"/>
+        <v>83</v>
+      </c>
+      <c r="C39" s="76"/>
       <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2883,9 +2903,9 @@
         <v>31</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="77"/>
+        <v>84</v>
+      </c>
+      <c r="C40" s="76"/>
       <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2893,287 +2913,307 @@
         <v>32</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="77"/>
+        <v>138</v>
+      </c>
+      <c r="C41" s="76"/>
       <c r="D41" s="75"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39" t="s">
+    <row r="42" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="78">
+        <v>33</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="44"/>
+      <c r="D42" s="75"/>
+    </row>
+    <row r="43" spans="1:4" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="78">
+        <v>34</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="44"/>
+      <c r="D43" s="75"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="38"/>
+      <c r="B44" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="48">
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="48">
         <v>1</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B45" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="77"/>
-      <c r="D43" s="31"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="48">
+      <c r="C45" s="76"/>
+      <c r="D45" s="31"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="48">
         <v>2</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B46" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="31"/>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="48">
+      <c r="C46" s="76"/>
+      <c r="D46" s="31"/>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="48">
         <v>3</v>
       </c>
-      <c r="B45" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="C45" s="77"/>
-      <c r="D45" s="31"/>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="48">
-        <v>4</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C46" s="77"/>
-      <c r="D46" s="31"/>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="48">
-        <v>5</v>
-      </c>
       <c r="B47" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="77"/>
+        <v>146</v>
+      </c>
+      <c r="C47" s="76"/>
       <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
+        <v>4</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="76"/>
+      <c r="D48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="48">
+        <v>5</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="76"/>
+      <c r="D49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="48">
         <v>6</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="77"/>
-      <c r="D48" s="31"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="48">
+      <c r="B50" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="76"/>
+      <c r="D50" s="31"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="48">
         <v>7</v>
       </c>
-      <c r="B49" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="77"/>
-      <c r="D49" s="31"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="48">
-        <v>8</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" s="77"/>
-      <c r="D50" s="31"/>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="48">
-        <v>9</v>
-      </c>
       <c r="B51" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="77"/>
+        <v>102</v>
+      </c>
+      <c r="C51" s="76"/>
       <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="77"/>
+        <v>36</v>
+      </c>
+      <c r="C52" s="76"/>
       <c r="D52" s="31"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C53" s="77"/>
+        <v>91</v>
+      </c>
+      <c r="C53" s="76"/>
       <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="77"/>
+        <v>68</v>
+      </c>
+      <c r="C54" s="76"/>
       <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="77"/>
+        <v>124</v>
+      </c>
+      <c r="C55" s="76"/>
       <c r="D55" s="31"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="77"/>
+        <v>69</v>
+      </c>
+      <c r="C56" s="76"/>
       <c r="D56" s="31"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="C57" s="76"/>
       <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="77"/>
+        <v>71</v>
+      </c>
+      <c r="C58" s="76"/>
       <c r="D58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" s="77"/>
+        <v>72</v>
+      </c>
+      <c r="C59" s="76"/>
       <c r="D59" s="31"/>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="77"/>
+        <v>74</v>
+      </c>
+      <c r="C60" s="76"/>
       <c r="D60" s="31"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
+        <v>17</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="76"/>
+      <c r="D61" s="31"/>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="48">
+        <v>18</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="76"/>
+      <c r="D62" s="31"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="48">
         <v>19</v>
       </c>
-      <c r="B61" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="C61" s="77"/>
-      <c r="D61" s="31"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="48">
+      <c r="B63" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="76"/>
+      <c r="D63" s="31"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="48">
         <v>20</v>
       </c>
-      <c r="B62" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="77"/>
-      <c r="D62" s="31"/>
-    </row>
-    <row r="63" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="38"/>
-      <c r="B63" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="45">
+      <c r="B64" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="76"/>
+      <c r="D64" s="31"/>
+    </row>
+    <row r="65" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="38"/>
+      <c r="B65" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="45">
         <v>1</v>
       </c>
-      <c r="B64" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" s="77"/>
-      <c r="D64" s="37"/>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="52">
-        <v>2</v>
-      </c>
-      <c r="B65" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" s="77"/>
-      <c r="D65" s="37"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="52">
-        <v>3</v>
-      </c>
-      <c r="B66" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="77"/>
+      <c r="B66" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="76"/>
       <c r="D66" s="37"/>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="52">
+        <v>2</v>
+      </c>
+      <c r="B67" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="76"/>
+      <c r="D67" s="37"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="52">
+        <v>3</v>
+      </c>
+      <c r="B68" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="76"/>
+      <c r="D68" s="37"/>
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="52">
         <v>4</v>
       </c>
-      <c r="B67" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C67" s="77"/>
-      <c r="D67" s="37"/>
-    </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="52">
+      <c r="B69" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="76"/>
+      <c r="D69" s="37"/>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="52">
         <v>5</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B70" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="77"/>
-      <c r="D68" s="37"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D63">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D65">
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C41 C43:C62 C64:C68">
-      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C43 C45:C64 C66:C70">
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3188,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,27 +3243,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3235,10 +3275,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3246,9 +3286,9 @@
         <v>1</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="77"/>
+        <v>103</v>
+      </c>
+      <c r="C9" s="76"/>
       <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,9 +3296,9 @@
         <v>2</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="77"/>
+        <v>125</v>
+      </c>
+      <c r="C10" s="76"/>
       <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,9 +3306,9 @@
         <v>3</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="77"/>
+        <v>105</v>
+      </c>
+      <c r="C11" s="76"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3276,9 +3316,9 @@
         <v>4</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="77"/>
+        <v>106</v>
+      </c>
+      <c r="C12" s="76"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3288,7 +3328,7 @@
       <c r="B13" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="77"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3298,7 +3338,7 @@
       <c r="B14" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="77"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3306,9 +3346,9 @@
         <v>7</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="77"/>
+        <v>126</v>
+      </c>
+      <c r="C15" s="76"/>
       <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3316,9 +3356,9 @@
         <v>8</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="77"/>
+        <v>130</v>
+      </c>
+      <c r="C16" s="76"/>
       <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,9 +3366,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="77"/>
+        <v>59</v>
+      </c>
+      <c r="C17" s="76"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3336,9 +3376,9 @@
         <v>10</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="77"/>
+        <v>61</v>
+      </c>
+      <c r="C18" s="76"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3346,9 +3386,9 @@
         <v>11</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C19" s="77"/>
+        <v>148</v>
+      </c>
+      <c r="C19" s="76"/>
       <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3356,9 +3396,9 @@
         <v>12</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="77"/>
+        <v>65</v>
+      </c>
+      <c r="C20" s="76"/>
       <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3366,49 +3406,49 @@
         <v>13</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="77"/>
+        <v>107</v>
+      </c>
+      <c r="C21" s="76"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="44">
         <v>14</v>
       </c>
-      <c r="B22" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="77"/>
+      <c r="B22" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="76"/>
       <c r="D22" s="37"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="44">
         <v>15</v>
       </c>
-      <c r="B23" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="77"/>
+      <c r="B23" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="76"/>
       <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="44">
         <v>16</v>
       </c>
-      <c r="B24" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="77"/>
+      <c r="B24" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="76"/>
       <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="44">
         <v>17</v>
       </c>
-      <c r="B25" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="77"/>
+      <c r="B25" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="76"/>
       <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3416,9 +3456,9 @@
         <v>18</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C26" s="77"/>
+        <v>148</v>
+      </c>
+      <c r="C26" s="76"/>
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,9 +3466,9 @@
         <v>19</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="77"/>
+        <v>131</v>
+      </c>
+      <c r="C27" s="76"/>
       <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,9 +3476,9 @@
         <v>20</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="77"/>
+        <v>41</v>
+      </c>
+      <c r="C28" s="76"/>
       <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3446,9 +3486,9 @@
         <v>21</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="77"/>
+        <v>85</v>
+      </c>
+      <c r="C29" s="76"/>
       <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3456,9 +3496,9 @@
         <v>22</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="C30" s="77"/>
+        <v>149</v>
+      </c>
+      <c r="C30" s="76"/>
       <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3466,9 +3506,9 @@
         <v>23</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="77"/>
+        <v>86</v>
+      </c>
+      <c r="C31" s="76"/>
       <c r="D31" s="49"/>
     </row>
     <row r="32" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3476,9 +3516,9 @@
         <v>24</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="77"/>
+        <v>139</v>
+      </c>
+      <c r="C32" s="76"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3496,7 +3536,7 @@
       <c r="B34" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="77"/>
+      <c r="C34" s="76"/>
       <c r="D34" s="37"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,9 +3544,9 @@
         <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="77"/>
+        <v>108</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="37"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3514,9 +3554,9 @@
         <v>4</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="77"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="76"/>
       <c r="D36" s="37"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3524,9 +3564,9 @@
         <v>5</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="77"/>
+        <v>128</v>
+      </c>
+      <c r="C37" s="76"/>
       <c r="D37" s="37"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3534,9 +3574,9 @@
         <v>6</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="77"/>
+        <v>62</v>
+      </c>
+      <c r="C38" s="76"/>
       <c r="D38" s="37"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3544,9 +3584,9 @@
         <v>7</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="77"/>
+        <v>121</v>
+      </c>
+      <c r="C39" s="76"/>
       <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,9 +3594,9 @@
         <v>8</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="77"/>
+        <v>150</v>
+      </c>
+      <c r="C40" s="76"/>
       <c r="D40" s="37"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3564,9 +3604,9 @@
         <v>10</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="77"/>
+        <v>68</v>
+      </c>
+      <c r="C41" s="76"/>
       <c r="D41" s="49"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,9 +3614,9 @@
         <v>12</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="77"/>
+        <v>69</v>
+      </c>
+      <c r="C42" s="76"/>
       <c r="D42" s="49"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,9 +3624,9 @@
         <v>13</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="C43" s="76"/>
       <c r="D43" s="49"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3594,9 +3634,9 @@
         <v>14</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="77"/>
+        <v>71</v>
+      </c>
+      <c r="C44" s="76"/>
       <c r="D44" s="49"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,9 +3644,9 @@
         <v>15</v>
       </c>
       <c r="B45" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="77"/>
+        <v>72</v>
+      </c>
+      <c r="C45" s="76"/>
       <c r="D45" s="56"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,9 +3654,9 @@
         <v>16</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="77"/>
+        <v>74</v>
+      </c>
+      <c r="C46" s="76"/>
       <c r="D46" s="44"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3624,9 +3664,9 @@
         <v>17</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="77"/>
+        <v>75</v>
+      </c>
+      <c r="C47" s="76"/>
       <c r="D47" s="46"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3634,9 +3674,9 @@
         <v>18</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="77"/>
+        <v>76</v>
+      </c>
+      <c r="C48" s="76"/>
       <c r="D48" s="46"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3644,9 +3684,9 @@
         <v>19</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="77"/>
+        <v>91</v>
+      </c>
+      <c r="C49" s="76"/>
       <c r="D49" s="49"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3654,9 +3694,9 @@
         <v>20</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="77"/>
+        <v>147</v>
+      </c>
+      <c r="C50" s="76"/>
       <c r="D50" s="49"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,9 +3704,9 @@
         <v>21</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="77"/>
+        <v>142</v>
+      </c>
+      <c r="C51" s="76"/>
       <c r="D51" s="49"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3682,9 +3722,9 @@
         <v>1</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="C53" s="77"/>
+        <v>136</v>
+      </c>
+      <c r="C53" s="76"/>
       <c r="D53" s="37"/>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3692,9 +3732,9 @@
         <v>2</v>
       </c>
       <c r="B54" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="77"/>
+        <v>38</v>
+      </c>
+      <c r="C54" s="76"/>
       <c r="D54" s="37"/>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3702,9 +3742,9 @@
         <v>3</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="77"/>
+        <v>39</v>
+      </c>
+      <c r="C55" s="76"/>
       <c r="D55" s="37"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,7 +3754,7 @@
       <c r="B56" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="77"/>
+      <c r="C56" s="76"/>
       <c r="D56" s="37"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,7 +3764,7 @@
       <c r="B57" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="77"/>
+      <c r="C57" s="76"/>
       <c r="D57" s="37"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,7 +3774,7 @@
       <c r="B58" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C58" s="77"/>
+      <c r="C58" s="76"/>
       <c r="D58" s="37"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3742,15 +3782,15 @@
         <v>7</v>
       </c>
       <c r="B59" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" s="77"/>
+        <v>40</v>
+      </c>
+      <c r="C59" s="76"/>
       <c r="D59" s="37"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="38"/>
       <c r="B60" s="39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
@@ -3760,9 +3800,9 @@
         <v>1</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="77"/>
+        <v>104</v>
+      </c>
+      <c r="C61" s="76"/>
       <c r="D61" s="37"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,7 +3812,7 @@
       <c r="B62" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="77"/>
+      <c r="C62" s="76"/>
       <c r="D62" s="49"/>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3780,9 +3820,9 @@
         <v>3</v>
       </c>
       <c r="B63" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" s="77"/>
+        <v>101</v>
+      </c>
+      <c r="C63" s="76"/>
       <c r="D63" s="49"/>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3792,7 +3832,7 @@
       <c r="B64" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="77"/>
+      <c r="C64" s="76"/>
       <c r="D64" s="49"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3800,9 +3840,9 @@
         <v>5</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C65" s="77"/>
+        <v>36</v>
+      </c>
+      <c r="C65" s="76"/>
       <c r="D65" s="49"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,9 +3850,9 @@
         <v>6</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="77"/>
+        <v>110</v>
+      </c>
+      <c r="C66" s="76"/>
       <c r="D66" s="56"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3820,9 +3860,9 @@
         <v>7</v>
       </c>
       <c r="B67" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" s="77"/>
+        <v>42</v>
+      </c>
+      <c r="C67" s="76"/>
       <c r="D67" s="56"/>
     </row>
   </sheetData>
@@ -3831,7 +3871,7 @@
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C32 C34:C51 C53:C59 C61:C67">
-      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3846,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,27 +3901,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3893,10 +3933,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3904,9 +3944,9 @@
         <v>1</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="77"/>
+        <v>151</v>
+      </c>
+      <c r="C10" s="76"/>
       <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3914,9 +3954,9 @@
         <v>2</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="77"/>
+        <v>43</v>
+      </c>
+      <c r="C11" s="76"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3924,9 +3964,9 @@
         <v>3</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="77"/>
+        <v>111</v>
+      </c>
+      <c r="C12" s="76"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3934,9 +3974,9 @@
         <v>4</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="77"/>
+        <v>44</v>
+      </c>
+      <c r="C13" s="76"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3944,29 +3984,29 @@
         <v>5</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="77"/>
+        <v>152</v>
+      </c>
+      <c r="C14" s="76"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>6</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="77"/>
+      <c r="B15" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="76"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
         <v>7</v>
       </c>
-      <c r="B16" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="77"/>
+      <c r="B16" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="76"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3976,7 +4016,7 @@
       <c r="B17" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="77"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,7 +4026,7 @@
       <c r="B18" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="77"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3994,9 +4034,9 @@
         <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="77"/>
+        <v>139</v>
+      </c>
+      <c r="C19" s="76"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4014,7 +4054,7 @@
       <c r="B21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="77"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,7 +4064,7 @@
       <c r="B22" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="77"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="37"/>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4032,9 +4072,9 @@
         <v>3</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="77"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="76"/>
       <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4042,9 +4082,9 @@
         <v>4</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="77"/>
+        <v>128</v>
+      </c>
+      <c r="C24" s="76"/>
       <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4052,9 +4092,9 @@
         <v>5</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="77"/>
+        <v>62</v>
+      </c>
+      <c r="C25" s="76"/>
       <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4062,9 +4102,9 @@
         <v>6</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="77"/>
+        <v>121</v>
+      </c>
+      <c r="C26" s="76"/>
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4072,9 +4112,9 @@
         <v>7</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="77"/>
+        <v>109</v>
+      </c>
+      <c r="C27" s="76"/>
       <c r="D27" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,9 +4122,9 @@
         <v>8</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="77"/>
+        <v>68</v>
+      </c>
+      <c r="C28" s="76"/>
       <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4092,9 +4132,9 @@
         <v>9</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="77"/>
+        <v>133</v>
+      </c>
+      <c r="C29" s="76"/>
       <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4102,9 +4142,9 @@
         <v>10</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="77"/>
+        <v>69</v>
+      </c>
+      <c r="C30" s="76"/>
       <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,9 +4152,9 @@
         <v>11</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="C31" s="76"/>
       <c r="D31" s="49"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,9 +4162,9 @@
         <v>12</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="77"/>
+        <v>71</v>
+      </c>
+      <c r="C32" s="76"/>
       <c r="D32" s="49"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4132,9 +4172,9 @@
         <v>13</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="77"/>
+        <v>72</v>
+      </c>
+      <c r="C33" s="76"/>
       <c r="D33" s="56"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,9 +4182,9 @@
         <v>14</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="77"/>
+        <v>74</v>
+      </c>
+      <c r="C34" s="76"/>
       <c r="D34" s="44"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,9 +4192,9 @@
         <v>15</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="77"/>
+        <v>75</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="46"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4162,9 +4202,9 @@
         <v>16</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="77"/>
+        <v>76</v>
+      </c>
+      <c r="C36" s="76"/>
       <c r="D36" s="46"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4172,9 +4212,9 @@
         <v>17</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="77"/>
+        <v>91</v>
+      </c>
+      <c r="C37" s="76"/>
       <c r="D37" s="49"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4182,9 +4222,9 @@
         <v>18</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="C38" s="77"/>
+        <v>147</v>
+      </c>
+      <c r="C38" s="76"/>
       <c r="D38" s="49"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4192,9 +4232,9 @@
         <v>19</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="77"/>
+        <v>142</v>
+      </c>
+      <c r="C39" s="76"/>
       <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4210,9 +4250,9 @@
         <v>1</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="77"/>
+        <v>132</v>
+      </c>
+      <c r="C41" s="76"/>
       <c r="D41" s="37"/>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4220,9 +4260,9 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="77"/>
+        <v>38</v>
+      </c>
+      <c r="C42" s="76"/>
       <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,7 +4272,7 @@
       <c r="B43" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="77"/>
+      <c r="C43" s="76"/>
       <c r="D43" s="37"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4242,7 +4282,7 @@
       <c r="B44" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="76"/>
       <c r="D44" s="37"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4250,9 +4290,9 @@
         <v>5</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="77"/>
+        <v>134</v>
+      </c>
+      <c r="C45" s="76"/>
       <c r="D45" s="37"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4260,15 +4300,15 @@
         <v>6</v>
       </c>
       <c r="B46" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="77"/>
+        <v>40</v>
+      </c>
+      <c r="C46" s="76"/>
       <c r="D46" s="37"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C47" s="38"/>
       <c r="D47" s="38"/>
@@ -4280,7 +4320,7 @@
       <c r="B48" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="77"/>
+      <c r="C48" s="76"/>
       <c r="D48" s="49"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4288,9 +4328,9 @@
         <v>2</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="77"/>
+        <v>63</v>
+      </c>
+      <c r="C49" s="76"/>
       <c r="D49" s="49"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4300,7 +4340,7 @@
       <c r="B50" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="77"/>
+      <c r="C50" s="76"/>
       <c r="D50" s="49"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4308,9 +4348,9 @@
         <v>4</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="77"/>
+        <v>39</v>
+      </c>
+      <c r="C51" s="76"/>
       <c r="D51" s="49"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4318,9 +4358,9 @@
         <v>5</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="77"/>
+        <v>36</v>
+      </c>
+      <c r="C52" s="76"/>
       <c r="D52" s="49"/>
     </row>
   </sheetData>
@@ -4329,7 +4369,7 @@
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C19 C21:C39 C41:C46 C48:C52">
-      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4343,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:C61"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4357,27 +4397,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -4389,10 +4429,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4400,9 +4440,9 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="77"/>
+        <v>46</v>
+      </c>
+      <c r="C9" s="76"/>
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4410,9 +4450,9 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="77"/>
+        <v>45</v>
+      </c>
+      <c r="C10" s="76"/>
       <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4420,9 +4460,9 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="77"/>
+        <v>153</v>
+      </c>
+      <c r="C11" s="76"/>
       <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,9 +4470,9 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="77"/>
+        <v>48</v>
+      </c>
+      <c r="C12" s="76"/>
       <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4440,9 +4480,9 @@
         <v>5</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="77"/>
+        <v>85</v>
+      </c>
+      <c r="C13" s="76"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4452,7 +4492,7 @@
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="77"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4462,7 +4502,7 @@
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="77"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4470,9 +4510,9 @@
         <v>8</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="77"/>
+        <v>47</v>
+      </c>
+      <c r="C16" s="76"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4480,9 +4520,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="77"/>
+        <v>154</v>
+      </c>
+      <c r="C17" s="76"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4490,9 +4530,9 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="77"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="76"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4500,9 +4540,9 @@
         <v>11</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="77"/>
+        <v>86</v>
+      </c>
+      <c r="C19" s="76"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4510,9 +4550,9 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="77"/>
+        <v>112</v>
+      </c>
+      <c r="C20" s="76"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4520,15 +4560,15 @@
         <v>13</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="77"/>
+        <v>139</v>
+      </c>
+      <c r="C21" s="76"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -4538,9 +4578,9 @@
         <v>1</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="77"/>
+        <v>51</v>
+      </c>
+      <c r="C23" s="76"/>
       <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4548,9 +4588,9 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="77"/>
+        <v>52</v>
+      </c>
+      <c r="C24" s="76"/>
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4558,9 +4598,9 @@
         <v>3</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="77"/>
+        <v>53</v>
+      </c>
+      <c r="C25" s="76"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4568,9 +4608,9 @@
         <v>4</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="77"/>
+        <v>155</v>
+      </c>
+      <c r="C26" s="76"/>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4578,9 +4618,9 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="77"/>
+        <v>49</v>
+      </c>
+      <c r="C27" s="76"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4598,7 +4638,7 @@
       <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="77"/>
+      <c r="C29" s="76"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4606,9 +4646,9 @@
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="77"/>
+        <v>108</v>
+      </c>
+      <c r="C30" s="76"/>
       <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4616,9 +4656,9 @@
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="77"/>
+        <v>35</v>
+      </c>
+      <c r="C31" s="76"/>
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4626,9 +4666,9 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="77"/>
+        <v>128</v>
+      </c>
+      <c r="C32" s="76"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4636,9 +4676,9 @@
         <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="77"/>
+        <v>62</v>
+      </c>
+      <c r="C33" s="76"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4646,9 +4686,9 @@
         <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="77"/>
+        <v>121</v>
+      </c>
+      <c r="C34" s="76"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,9 +4696,9 @@
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="77"/>
+        <v>150</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4666,9 +4706,9 @@
         <v>8</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="77"/>
+        <v>68</v>
+      </c>
+      <c r="C36" s="76"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4676,9 +4716,9 @@
         <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="77"/>
+        <v>133</v>
+      </c>
+      <c r="C37" s="76"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4686,9 +4726,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="77"/>
+        <v>69</v>
+      </c>
+      <c r="C38" s="76"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4696,9 +4736,9 @@
         <v>11</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="C39" s="76"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4706,9 +4746,9 @@
         <v>12</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="77"/>
+        <v>71</v>
+      </c>
+      <c r="C40" s="76"/>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4716,9 +4756,9 @@
         <v>13</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="77"/>
+        <v>72</v>
+      </c>
+      <c r="C41" s="76"/>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4726,9 +4766,9 @@
         <v>14</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="77"/>
+        <v>74</v>
+      </c>
+      <c r="C42" s="76"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4736,9 +4776,9 @@
         <v>15</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="77"/>
+        <v>75</v>
+      </c>
+      <c r="C43" s="76"/>
       <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:4" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4746,9 +4786,9 @@
         <v>16</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="77"/>
+        <v>91</v>
+      </c>
+      <c r="C44" s="76"/>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4756,9 +4796,9 @@
         <v>17</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="77"/>
+        <v>147</v>
+      </c>
+      <c r="C45" s="76"/>
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4766,9 +4806,9 @@
         <v>18</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="77"/>
+        <v>142</v>
+      </c>
+      <c r="C46" s="76"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4784,9 +4824,9 @@
         <v>1</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="77"/>
+        <v>136</v>
+      </c>
+      <c r="C48" s="76"/>
       <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4794,9 +4834,9 @@
         <v>2</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="77"/>
+        <v>38</v>
+      </c>
+      <c r="C49" s="76"/>
       <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4846,7 @@
       <c r="B50" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="77"/>
+      <c r="C50" s="76"/>
       <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4816,7 +4856,7 @@
       <c r="B51" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="77"/>
+      <c r="C51" s="76"/>
       <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4826,7 +4866,7 @@
       <c r="B52" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="77"/>
+      <c r="C52" s="76"/>
       <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4834,15 +4874,15 @@
         <v>6</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="77"/>
+        <v>40</v>
+      </c>
+      <c r="C53" s="76"/>
       <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="B54" s="39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
@@ -4854,7 +4894,7 @@
       <c r="B55" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="77"/>
+      <c r="C55" s="76"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4862,9 +4902,9 @@
         <v>2</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C56" s="77"/>
+        <v>135</v>
+      </c>
+      <c r="C56" s="76"/>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4872,9 +4912,9 @@
         <v>3</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="77"/>
+        <v>63</v>
+      </c>
+      <c r="C57" s="76"/>
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4884,7 +4924,7 @@
       <c r="B58" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="77"/>
+      <c r="C58" s="76"/>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4892,9 +4932,9 @@
         <v>5</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="77"/>
+        <v>76</v>
+      </c>
+      <c r="C59" s="76"/>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4902,9 +4942,9 @@
         <v>6</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" s="77"/>
+        <v>36</v>
+      </c>
+      <c r="C60" s="76"/>
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4912,9 +4952,9 @@
         <v>7</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="77"/>
+        <v>39</v>
+      </c>
+      <c r="C61" s="76"/>
       <c r="D61" s="5"/>
     </row>
   </sheetData>
@@ -4923,7 +4963,7 @@
       <formula1>"Major, Minor"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C21 C23:C27 C29:C46 C48:C53 C55:C61">
-      <formula1>"Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4935,21 +4975,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -4998,10 +5023,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5021,16 +5068,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055BC9AF-D8B7-4B16-B3B6-28577F5957CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504B26EA-C5E0-46B4-8CA4-AFD4010B6796}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>